<commit_message>
added wheel diameter, IRC, debugging safebytes
</commit_message>
<xml_diff>
--- a/helpers/Errors with coresponding codes.xlsx
+++ b/helpers/Errors with coresponding codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\log_analysis\log_analysis\src\helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBF2E48-A075-4735-9461-35C7E72821DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664FD79C-F943-4872-8E5C-9E2F30CFE2E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{393BC539-5651-4F97-AB2A-439B31DC9896}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{393BC539-5651-4F97-AB2A-439B31DC9896}"/>
   </bookViews>
   <sheets>
     <sheet name="Chybyové hlásenia" sheetId="1" r:id="rId1"/>
@@ -800,18 +800,18 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="100.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="144.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.23046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="144.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -825,7 +825,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>100</v>
       </c>
@@ -839,7 +839,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>101</v>
       </c>
@@ -853,7 +853,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>102</v>
       </c>
@@ -867,7 +867,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>103</v>
       </c>
@@ -878,7 +878,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>104</v>
       </c>
@@ -886,7 +886,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>105</v>
       </c>
@@ -897,7 +897,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>106</v>
       </c>
@@ -908,7 +908,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>107</v>
       </c>
@@ -922,7 +922,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>108</v>
       </c>
@@ -936,7 +936,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>109</v>
       </c>
@@ -950,7 +950,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>110</v>
       </c>
@@ -964,7 +964,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>111</v>
       </c>
@@ -975,7 +975,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>112</v>
       </c>
@@ -989,7 +989,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>113</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>114</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>115</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>116</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>200</v>
       </c>
@@ -1069,14 +1069,14 @@
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="9.15234375" style="1"/>
     <col min="2" max="2" width="104" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.53515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
         <v>82</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>44</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\02\TN_.log</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>45</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\03\PV_.log</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>46</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\09\OZP_.lo</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>47</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\10\AV_.log</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>48</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\11\EN_OZP_</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>49</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\02\PH_.log</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>50</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\03\AV_.log</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>51</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\08\EN_.log</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>52</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\11\MO_.log</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>53</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\12\VA_.log</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>54</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2015\02\IvB_.lo</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>55</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2015\04\IvB_.lo</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>56</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>57</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>58</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>59</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>60</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>61</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>62</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>63</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>64</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\02\AL_.log</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>65</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\03\IvB_.log</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>66</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\03\JD_.log</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>67</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\04\IvB_.log</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>68</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\04\VA_.LOG</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>69</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\05\AL_.log</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>70</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\05\EN_.log</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>71</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\05\MO_.log</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
         <v>72</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\05\RD_AP.LOG.txt</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
         <v>73</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\11\AL_.LOG</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>74</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2017\01\kvB_amw.log</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
         <v>75</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2017\06\IvB_.log</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
         <v>76</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2017\06\OZP28_.log</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
         <v>77</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2017\10\PH_.log</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
         <v>78</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2017\12\TU_.log</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
         <v>79</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2018\04\TU_MAP_DAM3G_20180411_105836.log nie je</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
         <v>80</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2019\09\VL_AP_2019-09.log</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
         <v>81</v>
       </c>
@@ -1634,18 +1634,18 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.53515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="21.1796875" customWidth="1"/>
-    <col min="4" max="4" width="17.81640625" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" customWidth="1"/>
-    <col min="6" max="6" width="14.81640625" customWidth="1"/>
-    <col min="7" max="7" width="23.26953125" customWidth="1"/>
+    <col min="3" max="3" width="21.15234375" customWidth="1"/>
+    <col min="4" max="4" width="17.84375" customWidth="1"/>
+    <col min="5" max="5" width="9.69140625" customWidth="1"/>
+    <col min="6" max="6" width="14.84375" customWidth="1"/>
+    <col min="7" max="7" width="23.23046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>109</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>116</v>
       </c>

</xml_diff>